<commit_message>
Updated UI layout and fixed bugs
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,79 +461,19 @@
           <t>shashikumar</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>190001055</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>190001055</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-10-08</t>
+          <t>2025-11-01</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>11:07:24</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>shashikumar</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>190001055</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2025-10-27</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>13:35:14</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>shashikumar</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>190001055</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2025-11-01</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>09:16:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>abhijit</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>210001001</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2025-11-01</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>09:16:42</t>
+          <t>10:44:25</t>
         </is>
       </c>
     </row>

</xml_diff>